<commit_message>
Pequeño arreglo en roundrobin y fix de test
</commit_message>
<xml_diff>
--- a/tests/roundrobin1.xlsx
+++ b/tests/roundrobin1.xlsx
@@ -353,7 +353,7 @@
   <dimension ref="B1:AI2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:S2"/>
+      <selection activeCell="Y7" sqref="Y7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="1.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -374,13 +374,13 @@
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="2">
+      <c r="T1" s="2">
         <v>1</v>
       </c>
-      <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
       <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>

</xml_diff>